<commit_message>
Update documentacion post reunion
</commit_message>
<xml_diff>
--- a/Ejemplos tablas reunion carma.xlsx
+++ b/Ejemplos tablas reunion carma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Carma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{597654C8-A7F2-4F84-A961-CC3ACDA95657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F04DD6-4464-4287-BCEA-07CF8814980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60AA8E3D-ABD6-4E76-BB22-A111E3B38A5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Lista de precios</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Servicios</t>
   </si>
   <si>
-    <t>Servicio</t>
-  </si>
-  <si>
     <t>Atencion Medica</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>En la carga de contratos si es area protegida se esconde la combo de personas y se habilita el valor para cargarlo a mano.</t>
+  </si>
+  <si>
+    <t>Empresa Prestadora</t>
+  </si>
+  <si>
+    <t>La lista de servicios es por empresa prestadora. Cuando un propsecto va a pasar a cliente le filtro la combo por empresa prestadora cargada.</t>
+  </si>
+  <si>
+    <t>Testeo CoVid</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9BBFAF-8267-401F-BF61-5A74574BD6B4}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,23 +456,26 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -488,71 +497,92 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
+      <c r="D3">
+        <v>350</v>
+      </c>
+      <c r="E3">
+        <v>450</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
-        <v>150</v>
-      </c>
-      <c r="C3">
-        <v>250</v>
-      </c>
-      <c r="D3">
-        <v>350</v>
-      </c>
-      <c r="E3">
-        <v>450</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-      <c r="C4">
-        <v>250</v>
-      </c>
-      <c r="D4">
-        <v>350</v>
-      </c>
-      <c r="E4">
-        <v>450</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="B5">
+        <v>220</v>
+      </c>
+      <c r="C5">
+        <v>280</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
+      <c r="E5">
+        <v>600</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>150</v>
-      </c>
-      <c r="C5">
-        <v>250</v>
-      </c>
-      <c r="D5">
-        <v>350</v>
-      </c>
-      <c r="E5">
-        <v>450</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -568,8 +598,14 @@
       <c r="E6">
         <v>450</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -586,7 +622,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -603,7 +639,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -620,7 +656,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -637,7 +673,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -654,7 +690,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -671,7 +707,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -688,7 +724,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -705,7 +741,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -722,7 +758,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -758,12 +794,17 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>